<commit_message>
synce screen + test
</commit_message>
<xml_diff>
--- a/confusion matrix - temp.xlsx
+++ b/confusion matrix - temp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\skybe\Dropbox (Personal)\courses\MTech Knowledge engineering\KE 5107 - Data Mining Methodology &amp; Methods\workshops\Bayesian\NaiveBayes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC2D118C-10A1-498B-8783-DBF5AB9B218C}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A60AFBCF-B824-4DC5-B8FE-E79D391742B9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15945" xr2:uid="{6A75B523-CFB1-4915-A7A6-396B1F886F56}"/>
   </bookViews>
@@ -452,7 +452,7 @@
   <dimension ref="C6:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+      <selection activeCell="E8" sqref="C6:K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -507,22 +507,22 @@
         <v>0</v>
       </c>
       <c r="E8" s="3">
-        <v>2146</v>
+        <v>2252</v>
       </c>
       <c r="F8" s="1">
-        <v>1925</v>
+        <v>1864</v>
       </c>
       <c r="G8" s="1">
-        <v>95</v>
+        <v>33</v>
       </c>
       <c r="H8" s="1">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="I8" s="1">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="J8" s="1">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="K8" s="1">
         <v>0</v>
@@ -534,22 +534,22 @@
         <v>1</v>
       </c>
       <c r="E9" s="1">
-        <v>1565</v>
+        <v>1581</v>
       </c>
       <c r="F9" s="3">
-        <v>4126</v>
+        <v>4142</v>
       </c>
       <c r="G9" s="1">
-        <v>264</v>
+        <v>98</v>
       </c>
       <c r="H9" s="1">
-        <v>176</v>
+        <v>206</v>
       </c>
       <c r="I9" s="1">
-        <v>34</v>
+        <v>97</v>
       </c>
       <c r="J9" s="1">
-        <v>14</v>
+        <v>55</v>
       </c>
       <c r="K9" s="1">
         <v>2</v>
@@ -561,25 +561,25 @@
         <v>2</v>
       </c>
       <c r="E10" s="1">
-        <v>170</v>
+        <v>141</v>
       </c>
       <c r="F10" s="1">
-        <v>644</v>
+        <v>688</v>
       </c>
       <c r="G10" s="3">
-        <v>155</v>
+        <v>43</v>
       </c>
       <c r="H10" s="1">
-        <v>84</v>
+        <v>129</v>
       </c>
       <c r="I10" s="1">
-        <v>16</v>
+        <v>50</v>
       </c>
       <c r="J10" s="1">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="K10" s="1">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="3:11" x14ac:dyDescent="0.45">
@@ -588,25 +588,25 @@
         <v>3</v>
       </c>
       <c r="E11" s="1">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="F11" s="1">
-        <v>316</v>
+        <v>305</v>
       </c>
       <c r="G11" s="1">
-        <v>84</v>
+        <v>48</v>
       </c>
       <c r="H11" s="3">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="I11" s="1">
-        <v>17</v>
+        <v>57</v>
       </c>
       <c r="J11" s="1">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="K11" s="1">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="3:11" x14ac:dyDescent="0.45">
@@ -615,22 +615,22 @@
         <v>4</v>
       </c>
       <c r="E12" s="1">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="F12" s="1">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="G12" s="1">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="H12" s="1">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="I12" s="3">
-        <v>64</v>
+        <v>41</v>
       </c>
       <c r="J12" s="1">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="K12" s="1">
         <v>1</v>
@@ -642,25 +642,25 @@
         <v>5</v>
       </c>
       <c r="E13" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F13" s="1">
         <v>33</v>
       </c>
       <c r="G13" s="1">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="H13" s="1">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="I13" s="1">
-        <v>7</v>
+        <v>28</v>
       </c>
       <c r="J13" s="3">
-        <v>51</v>
+        <v>24</v>
       </c>
       <c r="K13" s="1">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="3:11" x14ac:dyDescent="0.45">
@@ -669,25 +669,25 @@
         <v>6</v>
       </c>
       <c r="E14" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F14" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G14" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="H14" s="1">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="I14" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J14" s="1">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="K14" s="3">
-        <v>29</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
leave 1 out updated
</commit_message>
<xml_diff>
--- a/confusion matrix - temp.xlsx
+++ b/confusion matrix - temp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\skybe\Dropbox (Personal)\courses\MTech Knowledge engineering\KE 5107 - Data Mining Methodology &amp; Methods\workshops\Bayesian\NaiveBayes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A60AFBCF-B824-4DC5-B8FE-E79D391742B9}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30138EEF-6ED2-4E97-87D6-835C4A6A5D95}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15945" xr2:uid="{6A75B523-CFB1-4915-A7A6-396B1F886F56}"/>
   </bookViews>
@@ -452,7 +452,7 @@
   <dimension ref="C6:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="C6:K14"/>
+      <selection activeCell="M20" sqref="M19:N20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -507,22 +507,22 @@
         <v>0</v>
       </c>
       <c r="E8" s="3">
-        <v>2252</v>
+        <v>2181</v>
       </c>
       <c r="F8" s="1">
-        <v>1864</v>
+        <v>1896</v>
       </c>
       <c r="G8" s="1">
-        <v>33</v>
+        <v>93</v>
       </c>
       <c r="H8" s="1">
         <v>69</v>
       </c>
       <c r="I8" s="1">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="J8" s="1">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="K8" s="1">
         <v>0</v>
@@ -534,22 +534,22 @@
         <v>1</v>
       </c>
       <c r="E9" s="1">
-        <v>1581</v>
+        <v>1582</v>
       </c>
       <c r="F9" s="3">
-        <v>4142</v>
+        <v>4110</v>
       </c>
       <c r="G9" s="1">
-        <v>98</v>
+        <v>267</v>
       </c>
       <c r="H9" s="1">
-        <v>206</v>
+        <v>173</v>
       </c>
       <c r="I9" s="1">
-        <v>97</v>
+        <v>32</v>
       </c>
       <c r="J9" s="1">
-        <v>55</v>
+        <v>15</v>
       </c>
       <c r="K9" s="1">
         <v>2</v>
@@ -561,25 +561,25 @@
         <v>2</v>
       </c>
       <c r="E10" s="1">
-        <v>141</v>
+        <v>165</v>
       </c>
       <c r="F10" s="1">
-        <v>688</v>
+        <v>652</v>
       </c>
       <c r="G10" s="3">
-        <v>43</v>
+        <v>154</v>
       </c>
       <c r="H10" s="1">
-        <v>129</v>
+        <v>82</v>
       </c>
       <c r="I10" s="1">
-        <v>50</v>
+        <v>16</v>
       </c>
       <c r="J10" s="1">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="K10" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="3:11" x14ac:dyDescent="0.45">
@@ -588,25 +588,25 @@
         <v>3</v>
       </c>
       <c r="E11" s="1">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="F11" s="1">
-        <v>305</v>
+        <v>317</v>
       </c>
       <c r="G11" s="1">
-        <v>48</v>
+        <v>83</v>
       </c>
       <c r="H11" s="3">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="I11" s="1">
-        <v>57</v>
+        <v>19</v>
       </c>
       <c r="J11" s="1">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="K11" s="1">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="3:11" x14ac:dyDescent="0.45">
@@ -615,25 +615,25 @@
         <v>4</v>
       </c>
       <c r="E12" s="1">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="F12" s="1">
+        <v>57</v>
+      </c>
+      <c r="G12" s="1">
+        <v>22</v>
+      </c>
+      <c r="H12" s="1">
+        <v>35</v>
+      </c>
+      <c r="I12" s="3">
         <v>65</v>
       </c>
-      <c r="G12" s="1">
-        <v>12</v>
-      </c>
-      <c r="H12" s="1">
-        <v>46</v>
-      </c>
-      <c r="I12" s="3">
-        <v>41</v>
-      </c>
       <c r="J12" s="1">
-        <v>21</v>
+        <v>4</v>
       </c>
       <c r="K12" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="3:11" x14ac:dyDescent="0.45">
@@ -648,19 +648,19 @@
         <v>33</v>
       </c>
       <c r="G13" s="1">
+        <v>12</v>
+      </c>
+      <c r="H13" s="1">
+        <v>21</v>
+      </c>
+      <c r="I13" s="1">
         <v>5</v>
       </c>
-      <c r="H13" s="1">
-        <v>29</v>
-      </c>
-      <c r="I13" s="1">
-        <v>28</v>
-      </c>
       <c r="J13" s="3">
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="K13" s="1">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="3:11" x14ac:dyDescent="0.45">
@@ -669,25 +669,25 @@
         <v>6</v>
       </c>
       <c r="E14" s="1">
+        <v>0</v>
+      </c>
+      <c r="F14" s="1">
         <v>1</v>
-      </c>
-      <c r="F14" s="1">
-        <v>3</v>
       </c>
       <c r="G14" s="1">
         <v>5</v>
       </c>
       <c r="H14" s="1">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="I14" s="1">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="J14" s="1">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="K14" s="3">
-        <v>5</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>